<commit_message>
select automaticly the cup size and the rod size
</commit_message>
<xml_diff>
--- a/src/assets/implantsDataBase.xlsx
+++ b/src/assets/implantsDataBase.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sites\cyriaque.digitalsolutions.app\angular-file-uploading\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B919108C-5ECD-44E4-A771-134C626DC62E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40E8C3F5-0B36-4FCF-ABC6-0E2FE21264DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15300" yWindow="3528" windowWidth="13824" windowHeight="7176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -7062,9 +7062,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U834"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A251" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2:G2"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.59765625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
correct the offset (on display) between stem axis and diaphyseal axis
</commit_message>
<xml_diff>
--- a/src/assets/implantsDataBase.xlsx
+++ b/src/assets/implantsDataBase.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sites\cyriaque.digitalsolutions.app\angular-file-uploading\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40E8C3F5-0B36-4FCF-ABC6-0E2FE21264DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63E05D5F-9EAB-4E86-8986-36433EF2678C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30828" yWindow="-4404" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -7062,9 +7062,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U834"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="F2:G2"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A791" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P818" sqref="P818"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.59765625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>

</xml_diff>